<commit_message>
Cambios en la bd
</commit_message>
<xml_diff>
--- a/src/plantillas/modelo_cuentas.xlsx
+++ b/src/plantillas/modelo_cuentas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\pruebas con js\src\plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81ECDB21-19E1-45D8-A537-65FE2FCF1194}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C7F8AA4-947C-4536-A778-248C991C9E0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-17235" yWindow="2700" windowWidth="21600" windowHeight="11385" tabRatio="770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3915" yWindow="2325" windowWidth="21600" windowHeight="11385" tabRatio="770" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan de Cuentas" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1285" uniqueCount="601">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1286" uniqueCount="602">
   <si>
     <t>ACTIVO</t>
   </si>
@@ -1824,6 +1824,9 @@
   </si>
   <si>
     <t>6.1.4.01.04</t>
+  </si>
+  <si>
+    <t>saldo</t>
   </si>
 </sst>
 </file>
@@ -2278,9 +2281,9 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1:B379"/>
+  <dimension ref="A1:C379"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -2291,15 +2294,18 @@
     <col min="3" max="16384" width="11.42578125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5">
         <v>1</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="7" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>7</v>
       </c>
@@ -2307,7 +2313,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>8</v>
       </c>
@@ -2315,7 +2321,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
@@ -2323,7 +2329,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>10</v>
       </c>
@@ -2331,7 +2337,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>11</v>
       </c>
@@ -2339,7 +2345,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>13</v>
       </c>
@@ -2347,7 +2353,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>14</v>
       </c>
@@ -2355,7 +2361,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>15</v>
       </c>
@@ -2363,7 +2369,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
@@ -2371,7 +2377,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>49</v>
       </c>
@@ -2379,7 +2385,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>530</v>
       </c>
@@ -2387,7 +2393,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>531</v>
       </c>
@@ -2395,7 +2401,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>545</v>
       </c>
@@ -2403,7 +2409,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>532</v>
       </c>
@@ -2411,7 +2417,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>18</v>
       </c>
@@ -5064,14 +5070,14 @@
   <sheetPr codeName="Hoja4"/>
   <dimension ref="A1:B378"/>
   <sheetViews>
-    <sheetView topLeftCell="A212" workbookViewId="0">
-      <selection activeCell="A212" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A320" workbookViewId="0">
+      <selection activeCell="B262" sqref="B262"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="2.7109375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="49.42578125" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="16384" width="11.42578125" style="4"/>
   </cols>
   <sheetData>

</xml_diff>